<commit_message>
Commit code for the jenkins.. Ashot issue.
Thanks,
Ajit Nakum..
</commit_message>
<xml_diff>
--- a/Automation/Workspace/Odysseus_Product/src/main/java/testData/LocalAirData.xlsx
+++ b/Automation/Workspace/Odysseus_Product/src/main/java/testData/LocalAirData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15855" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13710" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
     <t>nyc</t>
   </si>
   <si>
-    <t>mia</t>
+    <t>bost</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>